<commit_message>
Actualización al plan general
</commit_message>
<xml_diff>
--- a/tspi/ciclo-2/plan2-20106065.xlsx
+++ b/tspi/ciclo-2/plan2-20106065.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="9660" yWindow="-45" windowWidth="9540" windowHeight="7365" tabRatio="400"/>
+    <workbookView xWindow="9660" yWindow="-45" windowWidth="9540" windowHeight="7365" tabRatio="400" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -781,7 +781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:ALY23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
@@ -1870,7 +1870,7 @@
       <c r="ALX2" s="4"/>
       <c r="ALY2" s="4"/>
     </row>
-    <row r="3" spans="1:1013" ht="38.25">
+    <row r="3" spans="1:1013" ht="63.75">
       <c r="A3" s="8">
         <v>25</v>
       </c>
@@ -4979,7 +4979,7 @@
       <c r="ALX5" s="4"/>
       <c r="ALY5" s="4"/>
     </row>
-    <row r="6" spans="1:1013" ht="38.25">
+    <row r="6" spans="1:1013" ht="51">
       <c r="A6" s="8">
         <v>28</v>
       </c>
@@ -6016,7 +6016,7 @@
       <c r="ALX6" s="4"/>
       <c r="ALY6" s="4"/>
     </row>
-    <row r="7" spans="1:1013" ht="38.25">
+    <row r="7" spans="1:1013" ht="25.5">
       <c r="A7" s="8">
         <v>29</v>
       </c>
@@ -7053,7 +7053,7 @@
       <c r="ALX7" s="4"/>
       <c r="ALY7" s="4"/>
     </row>
-    <row r="8" spans="1:1013" ht="38.25">
+    <row r="8" spans="1:1013" ht="25.5">
       <c r="A8" s="8">
         <v>30</v>
       </c>
@@ -9125,7 +9125,7 @@
       <c r="ALX9" s="4"/>
       <c r="ALY9" s="4"/>
     </row>
-    <row r="10" spans="1:1013" ht="38.25">
+    <row r="10" spans="1:1013" ht="25.5">
       <c r="A10" s="8">
         <v>32</v>
       </c>
@@ -17421,7 +17421,7 @@
       <c r="ALX17" s="4"/>
       <c r="ALY17" s="4"/>
     </row>
-    <row r="18" spans="1:1013" ht="38.25">
+    <row r="18" spans="1:1013" ht="25.5">
       <c r="A18" s="8">
         <v>40</v>
       </c>
@@ -17557,7 +17557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:1013" ht="38.25">
+    <row r="22" spans="1:1013" ht="25.5">
       <c r="A22" s="8">
         <v>44</v>
       </c>
@@ -17592,7 +17592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:1013" ht="38.25">
+    <row r="23" spans="1:1013" ht="51">
       <c r="A23" s="8">
         <v>45</v>
       </c>
@@ -17847,8 +17847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:K3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.85546875" defaultRowHeight="12.75"/>

</xml_diff>